<commit_message>
feat: add hobby's column
취미 테이블에 요약 이름 컬럼 추가
</commit_message>
<xml_diff>
--- a/src/main/resources/static/initData.xlsx
+++ b/src/main/resources/static/initData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaeminlee/Documents/Repository/MOKY4/hollang-weeks52-api-server/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaeminlee/Documents/Repository/MOKY4/hollang-weeks52-api-server/src/main/resources/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98554E6F-5BB8-D14C-A04D-D9682BEDBBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DA0764-6475-7B48-B8A5-82009AFD0C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="19980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="156">
   <si>
     <t>질문</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3072,42 +3072,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>어도비 인디자인</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>프로크리에이트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>굿노트 다이어리 꾸미기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>감성 사진 촬영</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>포토샵 디자인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PPT 실무 템플릿</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>어도비 일러스트레이트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>비주얼 씽킹</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>일러스트 정복하기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>카피라이팅 실습</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3116,26 +3088,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>프리미어 프로</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>브런치 작가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NFT 아트 제작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wix 웹사이트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>카카오톡 이모티콘 만들기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>인스타툰 제작</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3144,14 +3100,214 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>블로그 퍼스널 브랜딩</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
-    <t>default</t>
+    <t>편집 디자인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>디지털 드로잉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>굿노트 다이어리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감성 사진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실무 PPT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>굿즈 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일러스트 학습</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영상 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFT 아트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NFT에 대한 전반적인 이해와 작품 구상, 제작, 거래 과정을 경험해보세요. 디지털 아트의 새로운 패러다임인 NFT에 대해 배우고, 자신만의 NFT 아트를 직접 제작해보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어도비 인디자인으로 간단한 명함부터 문서 디자인까지 다양한 디자인 작업에 도전해보세요. 편집 디자인의 기본부터 전문가 수준까지 단계별로 알아보며 실습을 통해 직접 경험해보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로크리에이트의 기본 도형과 다양한 효과를 활용하여 나만의 그림과 애니메이션을 제작해보세요. 그림을 그리는 기초부터 디지털 드로잉에 필요한 기술까지 한번에 배울 수 있습니다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>굿노트 앱을 활용하여 아이패드로 일상을 기록하고, 다양한 용도로 활용해볼까요? 굿노트 기능으로 예쁜 글씨를 써보고 나만의 다이어리 템플릿과 스티커로 다꾸를 시작해봅시다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사진 찍기, 보정 및 포토 에세이 작성, SNS 포트폴리오 제작 등 여러 미션들을 통해 사진 촬영 및 편집 역량을 향상시켜보세요! 일상의 순간을 예술적으로 담아볼까요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>웹 이미지, SNS 이미지, 영화 포스터 제작 등 포토샵을 활용한 다양한 디자인을 배워보세요. 디자인의 기본 개념과 포토샵의 활용법을 학습하고 실제 디자인 작업을 진행해보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>표지, 목차, 본문 작성부터 인포그래픽, 슬라이드 마스터를 활용한 실무 PPT 템플릿 제작까지 경험해보세요. 프레젠테이션을 위한 기본적인 요소와 실무 PPT 제작 꿀팁을 배울 수 있습니다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어도비 일러스트의 펜 툴과 패스파인더를 활용하여 로고, 캐릭터 스케치 및 굿즈 시안 디자인 실습을 해보세요. 자신만의 브랜드를 만들어보고, 그에 맞는 굿즈 디자인을 직접 해보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비주얼 씽킹을 활용한 정보 정리부터 학습 내용 정리까지 다양한 비주얼 씽킹 경험을 쌓아보세요. 복잡한 정보를 시각적으로 정리하고 공유하는 방법을 배워보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일러스트의 기능을 사용하여 디자인부터 포스터 제작, 실무 디자인 도전 등 여러 결과물들을 만들어볼까요? 툴 사용법뿐만 아니라 실제 디자인 작업에서의 활용 방법도 배워봅시다!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>글쓰기와 카피라이팅에 대한 이해를 바탕으로 공감과 판매를 높일 수 있는 글감을 찾고 작성하는 방법을 배워보세요. 감성적인 글쓰기와 함께 효과적인 카피라이팅 기법을 배워보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스토리텔링을 통해 좋아하는 작품의 장르, 독자, 도입부 분석하고 나만의 스토리를 기획해보세요. 강력한 스토리를 만들어 내는 방법을 배우고, 사람들의 마음을 사로잡는 방법을 배워보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프리미어 프로를 활용하여 1분 자기소개 영상을 기획, 제작하고 유튜브에 업로드해보세요. 영상 편집의 기초를 배우고, 이를 활용하여 효과적으로 자기소개 영상을 제작하는 방법을 배워보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self Q&amp;A, 글감 준비, 롤 모델 분석 등 브런치 작가로서의 활동을 위한 준비 과정을 경험해보세요. 작가의 생각과 고민을 정리하고, 자신만의 글쓰기 스타일을 찾아보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>웹사이트 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wix를 사용하여 쇼핑몰 웹사이트 구축, 상품 등록 및 관리, 그리고 마케팅까지 진행해보세요. 웹사이트 제작의 기본을 배우고, 이를 활용하여 자신만의 웹사이트를 제작해 보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이모티콘 제작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이디어 구상부터 캐릭터 제작, 이모티콘 디지털 드로잉, 그리고 플랫폼 제안까지의 이모티콘 제작 전 과정을 체험해보세요. 카카오톡에서 자신만의 이모티콘을 제작해 보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인스타툰 시장 조사, 기획안 작성, 콘티 작성 및 표지 디자인까지 인스타툰 제작 전 과정을 체험해보세요. 웹툰의 기본 구조를 배우고, 그에 따라 나만의 인스타툰을 제작해보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사업계획서 작성부터 사업 구상, 사업성 증명, 주요 마일스톤 설정까지 사업을 위한 계획을 세우는 방법을 배워보세요. 실제 사업을 시작하기 전에 필요한 모든 과정을 체험하고 배워보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>블로그 브랜딩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>블로그를 운영하는 계획을 세우고, 콘텐츠를 업로드하여 블로그를 활용하는 능력을 향상시키세요. 자신만의 브랜드를 구축하고, 그 브랜드를 표현하는 방법을 배워보세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adobe InDesign으로 편집 디자인 시작하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로크리에이트로 시작하는 디지털 드로잉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>굿노트 앱으로 다이어리 꾸미기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일상을 영화처럼 감성 사진 촬영하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Photoshop으로 디자인 시작하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPT 실무 템플릿 직접 만들어보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adobe illustrator로 나만의 굿즈 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>손으로 정리하는 생각 비주얼 씽킹 시작하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3주만에 일러스트 정복하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>콘텐츠 기획력 기르기: 카피라이팅 실습</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사람들을 사로잡는 스토리텔링 시작하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프리미어 프로로 1분 자기소개 영상 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>브런치 작가 도전하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나만의 NFT 아트 제작하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wix로 나만의 웹사이트 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카카오톡 이모티콘 출시하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘나가는 인스타툰 제작하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>첫 사업계획서 도전하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>블로그로 퍼스널 브랜딩 시작하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요약 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원본 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3334,6 +3490,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3797,333 +3957,394 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" thickBot="1">
+    <row r="1" spans="1:5" ht="19" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>154</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="76">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="76">
+      <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="76">
+      <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="76">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="19">
-      <c r="A2" t="s">
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="76">
+      <c r="A6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19">
-      <c r="A3" t="s">
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="76">
+      <c r="A7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="76">
+      <c r="A8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="76">
+      <c r="A9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="19">
-      <c r="A4" t="s">
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="76">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="76">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="19">
-      <c r="A5" t="s">
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="76">
+      <c r="A12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="19">
-      <c r="A6" t="s">
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="76">
+      <c r="A13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="76">
+      <c r="A14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="19">
-      <c r="A7" t="s">
+      <c r="C14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="76">
+      <c r="A15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="76">
+      <c r="A16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="76">
+      <c r="A17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="76">
+      <c r="A18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="19">
-      <c r="A8" t="s">
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="76">
+      <c r="A19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="19">
-      <c r="A9" t="s">
+      <c r="C19" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="19">
-      <c r="A10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="19">
-      <c r="A11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="19">
-      <c r="A12" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="19">
-      <c r="A13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="19">
-      <c r="A14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="19">
-      <c r="A15" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="19">
-      <c r="A16" t="s">
-        <v>109</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="19">
-      <c r="A17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="19">
-      <c r="A18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="19">
-      <c r="A19" t="s">
-        <v>112</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="19">
+      <c r="D19" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="76">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>132</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="B29" s="6"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="B32" s="6"/>
     </row>
     <row r="33" spans="2:2">
@@ -4135,6 +4356,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix: revise init data path and strategy
기본 데이터 경로와 전략 수정
</commit_message>
<xml_diff>
--- a/src/main/resources/static/initData.xlsx
+++ b/src/main/resources/static/initData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaeminlee/Documents/Repository/MOKY4/hollang-weeks52-api-server/src/main/resources/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DA0764-6475-7B48-B8A5-82009AFD0C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F39353-1A04-5049-B4A4-4610DB8D0FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="175">
   <si>
     <t>질문</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -3100,9 +3100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>default</t>
-  </si>
-  <si>
     <t>편집 디자인</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3312,6 +3309,86 @@
   </si>
   <si>
     <t>요약정보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>editorial-design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>digital-drawing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>goodnote-diary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>emotional-picture</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>photoshop-design</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>practical-ppt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>goods-production</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>visual-thinking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>illustration-learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>copywriting-practice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storytelling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>video-production</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brunch-writer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nft-art</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>creating-website</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>making-emoticons</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>production-of-instatoon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>preparation-of-business-plan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blog-branding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>준비중</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3490,10 +3567,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3959,8 +4032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -3969,17 +4042,18 @@
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19" thickBot="1">
       <c r="A1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>13</v>
@@ -3990,325 +4064,325 @@
     </row>
     <row r="2" spans="1:5" ht="76">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="76">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="76">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="76">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="76">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>95</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="76">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="76">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E8" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="76">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>96</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="76">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="76">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="76">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>98</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
-        <v>102</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="76">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E13" t="s">
-        <v>102</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="76">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>99</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="76">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C15" t="s">
-        <v>102</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>112</v>
-      </c>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="76">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C16" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>127</v>
-      </c>
       <c r="E16" t="s">
-        <v>102</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="76">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C17" t="s">
-        <v>102</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>129</v>
-      </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="76">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>100</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E18" t="s">
-        <v>102</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="76">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="76">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C20" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>133</v>
-      </c>
       <c r="E20" t="s">
-        <v>102</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:5">

</xml_diff>

<commit_message>
docs: fix duplicated test answer
</commit_message>
<xml_diff>
--- a/src/main/resources/static/initData.xlsx
+++ b/src/main/resources/static/initData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\SWYG\오오칠팔구\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaeminlee/Documents/Repository/MOKY4/hollang-weeks52-api-server/src/main/resources/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715BCFD2-5743-7A4B-8A51-2B2599428B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="756" windowWidth="34560" windowHeight="19980" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -1498,10 +1499,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>복권을 사야 하나? 바로 검색한다신기한 꿈이네. 뒷이야기는 뭐지?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>신기한 꿈이네. 뒷이야기는 뭐지?</t>
   </si>
   <si>
@@ -2753,11 +2750,15 @@
     <t>글쓰기 능력과 자신을 표현 할 수 있는 능력을 높일 수 있는 블로그 퍼스널 브랜딩을 추천해요</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
+  <si>
+    <t>복권을 사야 하나? 바로 검색한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="17">
     <font>
       <sz val="12"/>
@@ -2960,7 +2961,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3011,9 +3012,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -3347,21 +3345,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="19.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="35.08984375" customWidth="1"/>
-    <col min="2" max="2" width="26.6328125" customWidth="1"/>
-    <col min="3" max="3" width="69.26953125" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="69.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24.6" thickBot="1">
+    <row r="1" spans="1:3" ht="23" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3372,7 +3370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="76.8">
+    <row r="2" spans="1:3" ht="40">
       <c r="A2" s="13" t="s">
         <v>126</v>
       </c>
@@ -3383,7 +3381,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="38.4">
+    <row r="3" spans="1:3" ht="40">
       <c r="A3" s="13" t="s">
         <v>129</v>
       </c>
@@ -3394,7 +3392,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57.6">
+    <row r="4" spans="1:3" ht="40">
       <c r="A4" s="13" t="s">
         <v>132</v>
       </c>
@@ -3405,7 +3403,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="38.4">
+    <row r="5" spans="1:3" ht="40">
       <c r="A5" s="13" t="s">
         <v>135</v>
       </c>
@@ -3416,7 +3414,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="38.4">
+    <row r="6" spans="1:3" ht="40">
       <c r="A6" s="13" t="s">
         <v>138</v>
       </c>
@@ -3427,81 +3425,81 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="57.6">
+    <row r="7" spans="1:3" ht="60">
       <c r="A7" s="13" t="s">
         <v>141</v>
       </c>
       <c r="B7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" t="s">
         <v>142</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="40">
+      <c r="A8" s="13" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="38.4">
-      <c r="A8" s="13" t="s">
+      <c r="B8" t="s">
         <v>144</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>145</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="40">
+      <c r="A9" s="13" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="38.4">
-      <c r="A9" s="13" t="s">
+      <c r="B9" t="s">
         <v>147</v>
-      </c>
-      <c r="B9" t="s">
-        <v>148</v>
       </c>
       <c r="C9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="57.6">
+    <row r="10" spans="1:3" ht="60">
       <c r="A10" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="C10" t="s">
         <v>150</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="40">
+      <c r="A11" s="13" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="57.6">
-      <c r="A11" s="13" t="s">
+      <c r="B11" t="s">
         <v>152</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>153</v>
       </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="40">
+      <c r="A12" s="13" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="38.4">
-      <c r="A12" s="13" t="s">
+      <c r="B12" t="s">
         <v>155</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>156</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="60">
+      <c r="A13" s="13" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="57.6">
-      <c r="A13" s="13" t="s">
+      <c r="B13" t="s">
         <v>158</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>159</v>
-      </c>
-      <c r="C13" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3511,471 +3509,471 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="19.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="38.453125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="24" style="20" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="24" style="19" customWidth="1"/>
     <col min="3" max="3" width="64" style="16" customWidth="1"/>
-    <col min="4" max="4" width="40.453125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="26.54296875" style="20" customWidth="1"/>
-    <col min="7" max="16384" width="10.81640625" style="20"/>
+    <col min="4" max="4" width="40.42578125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="10.85546875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.8" thickBot="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:6" ht="19" thickBot="1">
+      <c r="A1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="76.8">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:6" ht="76">
+      <c r="A2" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="76">
+      <c r="A3" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="76">
+      <c r="A4" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="76">
+      <c r="A5" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="76.8">
-      <c r="A3" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="76.8">
-      <c r="A4" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="15" t="s">
+      <c r="D5" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="76">
+      <c r="A6" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="76">
+      <c r="A7" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="76">
+      <c r="A8" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="76">
+      <c r="A9" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="76">
+      <c r="A10" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" s="20" t="s">
+      <c r="D10" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="76.8">
-      <c r="A5" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="20" t="s">
+    <row r="11" spans="1:6" ht="76">
+      <c r="A11" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="76.8">
-      <c r="A6" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" s="20" t="s">
+    <row r="12" spans="1:6" ht="76">
+      <c r="A12" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="76.8">
-      <c r="A7" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="F7" s="20" t="s">
+    <row r="13" spans="1:6" ht="76">
+      <c r="A13" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="76.8">
-      <c r="A8" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F8" s="20" t="s">
+    <row r="14" spans="1:6" ht="76">
+      <c r="A14" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="76.8">
-      <c r="A9" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F9" s="20" t="s">
+    <row r="15" spans="1:6" ht="76">
+      <c r="A15" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="76.8">
-      <c r="A10" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="F10" s="20" t="s">
+    <row r="16" spans="1:6" ht="76">
+      <c r="A16" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="76.8">
-      <c r="A11" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="15" t="s">
+    <row r="17" spans="1:6" ht="76">
+      <c r="A17" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="76">
+      <c r="A18" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="F11" s="20" t="s">
+      <c r="D18" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="76.8">
-      <c r="A12" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="F12" s="20" t="s">
+    <row r="19" spans="1:6" ht="76">
+      <c r="A19" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="96">
-      <c r="A13" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="20" t="s">
+    <row r="20" spans="1:6" ht="76">
+      <c r="A20" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="76.8">
-      <c r="A14" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="F14" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="76.8">
-      <c r="A15" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="76.8">
-      <c r="A16" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="76.8">
-      <c r="A17" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="76.8">
-      <c r="A18" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="76.8">
-      <c r="A19" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="76.8">
-      <c r="A20" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>123</v>
-      </c>
-    </row>
     <row r="21" spans="1:6">
-      <c r="B21" s="21"/>
+      <c r="B21" s="20"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="B22" s="21"/>
+      <c r="B22" s="20"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="B23" s="21"/>
+      <c r="B23" s="20"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="B24" s="21"/>
+      <c r="B24" s="20"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="B25" s="21"/>
+      <c r="B25" s="20"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="B26" s="21"/>
+      <c r="B26" s="20"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="B27" s="21"/>
+      <c r="B27" s="20"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="B28" s="21"/>
+      <c r="B28" s="20"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="B29" s="21"/>
+      <c r="B29" s="20"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="B30" s="21"/>
+      <c r="B30" s="20"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="B31" s="21"/>
+      <c r="B31" s="20"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="B32" s="21"/>
+      <c r="B32" s="20"/>
     </row>
     <row r="33" spans="2:2">
-      <c r="B33" s="21"/>
+      <c r="B33" s="20"/>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="21"/>
+      <c r="B34" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3983,25 +3981,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="19.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="34.81640625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.8" thickBot="1">
+    <row r="1" spans="1:6" ht="19" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>16</v>
@@ -4016,12 +4014,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.6">
+    <row r="2" spans="1:6" ht="57">
       <c r="A2" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -4036,12 +4034,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="76.8">
+    <row r="3" spans="1:6" ht="76">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -4056,7 +4054,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57.6">
+    <row r="4" spans="1:6" ht="57">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -4076,12 +4074,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="57.6">
+    <row r="5" spans="1:6" ht="57">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -4096,12 +4094,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="57.6">
+    <row r="6" spans="1:6" ht="57">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -4116,12 +4114,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="57.6">
+    <row r="7" spans="1:6" ht="57">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -4136,7 +4134,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="76.8">
+    <row r="8" spans="1:6" ht="76">
       <c r="A8" s="8" t="s">
         <v>33</v>
       </c>
@@ -4156,12 +4154,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="57.6">
+    <row r="9" spans="1:6" ht="57">
       <c r="A9" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -4176,12 +4174,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="57.6">
+    <row r="10" spans="1:6" ht="57">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -4196,12 +4194,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="57.6">
+    <row r="11" spans="1:6" ht="57">
       <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
@@ -4216,12 +4214,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="76.8">
+    <row r="12" spans="1:6" ht="76">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
@@ -4236,12 +4234,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="76.8">
+    <row r="13" spans="1:6" ht="76">
       <c r="A13" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -4256,12 +4254,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="57.6">
+    <row r="14" spans="1:6" ht="57">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
         <v>29</v>
@@ -4276,12 +4274,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="76.8">
+    <row r="15" spans="1:6" ht="76">
       <c r="A15" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -4296,12 +4294,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="76.8">
+    <row r="16" spans="1:6" ht="76">
       <c r="A16" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>163</v>
       </c>
       <c r="C16" t="s">
         <v>31</v>
@@ -4316,12 +4314,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="76.8">
+    <row r="17" spans="1:6" ht="76">
       <c r="A17" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C17" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
feat: add hobby content url data
</commit_message>
<xml_diff>
--- a/src/main/resources/static/initData.xlsx
+++ b/src/main/resources/static/initData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaeminlee/Documents/Repository/MOKY4/hollang-weeks52-api-server/src/main/resources/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715BCFD2-5743-7A4B-8A51-2B2599428B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664D1284-8199-4542-89C7-042C89FF143C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="214">
   <si>
     <t>질문</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -547,13 +547,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://weeks52.me</t>
-  </si>
-  <si>
-    <t>https://weeks52.me</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>뭐야 대체 어케 했노</t>
   </si>
   <si>
@@ -2752,6 +2745,82 @@
   </si>
   <si>
     <t>복권을 사야 하나? 바로 검색한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=2&amp;productid=1688516148774x372879713149911040</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=2&amp;productid=1688476268166x847358910071046100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=2&amp;productid=1688546014460x934263405997719600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=1&amp;productid=1688484025726x518312023756111900</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=2&amp;productid=1688567902779x351167402681040900</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=2&amp;productid=1688467976224x979184356179312600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=2&amp;productid=1688526536221x947248170721083400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=1&amp;productid=1688458442181x318366658459336700</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=2&amp;productid=1688439254408x193038696549974000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=2&amp;productid=1688455942365x168647349289353200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=1&amp;productid=1688479342851x664678732629016600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=1&amp;productid=1688538816839x494271123231342600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=1&amp;productid=1688523489520x330385813034237950</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=1&amp;productid=1688512071571x417458534779453440</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=1&amp;productid=1688450507825x583145737120645100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=1&amp;productid=1688510916678x695001630222843900</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=2&amp;productid=1688458543976x219199250884722700</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=2&amp;productid=1688458354215x474020676765745150</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://weeks52.me/?section=productdetail&amp;categorynum=1&amp;productid=1688476272022x578730520215552000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2759,7 +2828,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2875,15 +2944,6 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2961,7 +3021,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3025,10 +3085,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3348,7 +3405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -3372,134 +3429,134 @@
     </row>
     <row r="2" spans="1:3" ht="40">
       <c r="A2" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" t="s">
         <v>126</v>
-      </c>
-      <c r="B2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="40">
       <c r="A3" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="B3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="40">
       <c r="A4" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
         <v>132</v>
-      </c>
-      <c r="B4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="40">
       <c r="A5" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" t="s">
         <v>135</v>
-      </c>
-      <c r="B5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="40">
       <c r="A6" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" t="s">
         <v>138</v>
-      </c>
-      <c r="B6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60">
       <c r="A7" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="40">
       <c r="A8" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" t="s">
         <v>143</v>
-      </c>
-      <c r="B8" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="40">
       <c r="A9" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60">
       <c r="A10" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" t="s">
         <v>148</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C10" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="40">
       <c r="A11" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" t="s">
         <v>151</v>
-      </c>
-      <c r="B11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="40">
       <c r="A12" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" t="s">
         <v>154</v>
-      </c>
-      <c r="B12" t="s">
-        <v>155</v>
-      </c>
-      <c r="C12" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="60">
       <c r="A13" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" t="s">
         <v>157</v>
-      </c>
-      <c r="B13" t="s">
-        <v>158</v>
-      </c>
-      <c r="C13" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3512,8 +3569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18"/>
@@ -3523,7 +3580,7 @@
     <col min="3" max="3" width="64" style="16" customWidth="1"/>
     <col min="4" max="4" width="40.42578125" style="19" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="26.5703125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="94.7109375" style="19" customWidth="1"/>
     <col min="7" max="16384" width="10.85546875" style="19"/>
   </cols>
   <sheetData>
@@ -3555,7 +3612,7 @@
         <v>50</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>60</v>
@@ -3564,7 +3621,7 @@
         <v>103</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>124</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="76">
@@ -3575,7 +3632,7 @@
         <v>51</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>61</v>
@@ -3583,8 +3640,8 @@
       <c r="E3" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="22" t="s">
-        <v>124</v>
+      <c r="F3" s="21" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="76">
@@ -3595,7 +3652,7 @@
         <v>52</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>62</v>
@@ -3603,8 +3660,8 @@
       <c r="E4" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>123</v>
+      <c r="F4" s="21" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="76">
@@ -3615,7 +3672,7 @@
         <v>53</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>63</v>
@@ -3623,8 +3680,8 @@
       <c r="E5" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="19" t="s">
-        <v>123</v>
+      <c r="F5" s="21" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="76">
@@ -3635,7 +3692,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>64</v>
@@ -3643,8 +3700,8 @@
       <c r="E6" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>123</v>
+      <c r="F6" s="21" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="76">
@@ -3655,7 +3712,7 @@
         <v>54</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>65</v>
@@ -3663,8 +3720,8 @@
       <c r="E7" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>123</v>
+      <c r="F7" s="21" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="76">
@@ -3675,7 +3732,7 @@
         <v>55</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>66</v>
@@ -3683,8 +3740,8 @@
       <c r="E8" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>123</v>
+      <c r="F8" s="21" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="76">
@@ -3695,7 +3752,7 @@
         <v>44</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D9" s="20" t="s">
         <v>67</v>
@@ -3703,8 +3760,8 @@
       <c r="E9" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F9" s="19" t="s">
-        <v>123</v>
+      <c r="F9" s="21" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="76">
@@ -3715,7 +3772,7 @@
         <v>56</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>68</v>
@@ -3723,8 +3780,8 @@
       <c r="E10" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F10" s="19" t="s">
-        <v>123</v>
+      <c r="F10" s="21" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="76">
@@ -3735,7 +3792,7 @@
         <v>45</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>69</v>
@@ -3743,8 +3800,8 @@
       <c r="E11" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>123</v>
+      <c r="F11" s="21" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="76">
@@ -3755,7 +3812,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>70</v>
@@ -3763,8 +3820,8 @@
       <c r="E12" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>123</v>
+      <c r="F12" s="21" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="76">
@@ -3775,7 +3832,7 @@
         <v>57</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>71</v>
@@ -3783,8 +3840,8 @@
       <c r="E13" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>123</v>
+      <c r="F13" s="21" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="76">
@@ -3795,7 +3852,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D14" s="20" t="s">
         <v>72</v>
@@ -3803,8 +3860,8 @@
       <c r="E14" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="F14" s="19" t="s">
-        <v>123</v>
+      <c r="F14" s="21" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="76">
@@ -3815,7 +3872,7 @@
         <v>58</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>59</v>
@@ -3823,8 +3880,8 @@
       <c r="E15" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="19" t="s">
-        <v>123</v>
+      <c r="F15" s="21" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="76">
@@ -3835,7 +3892,7 @@
         <v>73</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>74</v>
@@ -3843,8 +3900,8 @@
       <c r="E16" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="F16" s="19" t="s">
-        <v>123</v>
+      <c r="F16" s="21" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="76">
@@ -3855,7 +3912,7 @@
         <v>75</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>76</v>
@@ -3863,8 +3920,8 @@
       <c r="E17" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="19" t="s">
-        <v>123</v>
+      <c r="F17" s="21" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="76">
@@ -3875,7 +3932,7 @@
         <v>48</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>77</v>
@@ -3883,8 +3940,8 @@
       <c r="E18" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="19" t="s">
-        <v>123</v>
+      <c r="F18" s="21" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="76">
@@ -3895,7 +3952,7 @@
         <v>49</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>78</v>
@@ -3903,8 +3960,8 @@
       <c r="E19" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="F19" s="19" t="s">
-        <v>123</v>
+      <c r="F19" s="21" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="76">
@@ -3915,7 +3972,7 @@
         <v>79</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>80</v>
@@ -3923,8 +3980,8 @@
       <c r="E20" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="F20" s="19" t="s">
-        <v>123</v>
+      <c r="F20" s="21" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3972,8 +4029,25 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{EA658F5A-5EEE-1745-80D4-3D5D1A0592B1}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{7565631A-74A1-DB4D-9A33-99C221DAE8DD}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{E95015C1-7326-9241-BEF0-0D0DA7E80BB2}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{CF7FD437-F269-2C4D-A7E8-DEBCAC15035B}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{C2205D33-0611-6346-98CE-04F60966239F}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{68A67EEB-19A3-D242-A874-7FA805F1BEDD}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{735BA1A6-9D9B-0B4A-B823-24D399AF2188}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{D4C4F614-FCC1-3F4E-AC51-CEE89DEB975F}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{60814624-F944-274F-9200-CCE703A72B43}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{6C9C319D-780D-554D-87D3-79C310043BD0}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{F6FDD8A8-84D5-C04E-93E7-C98B36F7988E}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{7B33B788-56EA-6E4D-AC29-87A8A3728784}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{79E42046-20FB-8B4D-A145-3826D5DE1205}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{382002CB-C6A6-2C4A-8454-E5559CA4EC70}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{61593CB7-C53E-154A-B2F0-42879F46CC01}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{0C5F9170-19F4-4141-AD3B-BAB6C853474C}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{338C5FA4-641E-554D-A30E-9876212B213B}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{313ADDBE-E90D-2740-9D38-73276F6F7979}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{EE5311AB-AC3B-F042-A12C-9351FE7A6D55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3999,7 +4073,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>16</v>
@@ -4019,7 +4093,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -4039,7 +4113,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -4079,7 +4153,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -4099,7 +4173,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -4119,7 +4193,7 @@
         <v>38</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -4156,10 +4230,10 @@
     </row>
     <row r="9" spans="1:6" ht="57">
       <c r="A9" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -4179,7 +4253,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -4199,7 +4273,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
@@ -4219,7 +4293,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
         <v>27</v>
@@ -4239,7 +4313,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
@@ -4259,7 +4333,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C14" t="s">
         <v>29</v>
@@ -4279,7 +4353,7 @@
         <v>36</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -4296,10 +4370,10 @@
     </row>
     <row r="16" spans="1:6" ht="76">
       <c r="A16" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
         <v>31</v>
@@ -4319,7 +4393,7 @@
         <v>37</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
         <v>32</v>

</xml_diff>